<commit_message>
Completando as atividades de teste da NN
</commit_message>
<xml_diff>
--- a/docs/CRONOGRAMA - Projeto Coruja.xlsx
+++ b/docs/CRONOGRAMA - Projeto Coruja.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\pedro\PI-Coruja\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6764A0B0-7765-4D1B-BB66-64B3BB0BC232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRONOGRAMA Modelo" sheetId="3" r:id="rId1"/>
@@ -13,8 +19,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'CRONOGRAMA Modelo'!$B$1:$S$24</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -131,12 +137,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +231,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -420,7 +433,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,6 +568,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,14 +600,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -896,24 +910,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
@@ -923,45 +937,45 @@
     <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" s="5" customFormat="1" ht="25.8">
+    <row r="2" spans="2:19" s="5" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="2:19" s="5" customFormat="1" ht="25.8">
+    <row r="3" spans="2:19" s="5" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="2:19" ht="14.4">
+    <row r="4" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="2:19" ht="17.399999999999999">
+    <row r="5" spans="2:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-    </row>
-    <row r="6" spans="2:19" ht="14.4">
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="2:19" s="1" customFormat="1" ht="14.4">
+    <row r="7" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
@@ -993,11 +1007,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B8" s="67" t="s">
+    <row r="8" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="69" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -1021,9 +1035,9 @@
       <c r="R8" s="32"/>
       <c r="S8" s="33"/>
     </row>
-    <row r="9" spans="2:19" s="1" customFormat="1" ht="14.4">
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
+    <row r="9" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="30" t="s">
         <v>11</v>
       </c>
@@ -1073,10 +1087,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:19" s="1" customFormat="1" ht="14.4">
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="71"/>
+    <row r="10" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="22">
         <v>45875</v>
       </c>
@@ -1136,11 +1150,11 @@
         <v>45980</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B11" s="62" t="s">
+    <row r="11" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="27" t="s">
@@ -1162,9 +1176,9 @@
       <c r="R11" s="44"/>
       <c r="S11" s="45"/>
     </row>
-    <row r="12" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B12" s="63"/>
-      <c r="C12" s="65"/>
+    <row r="12" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
@@ -1184,11 +1198,11 @@
       <c r="R12" s="44"/>
       <c r="S12" s="45"/>
     </row>
-    <row r="13" spans="2:19" ht="14.4">
-      <c r="B13" s="62" t="s">
+    <row r="13" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -1210,9 +1224,9 @@
       <c r="R13" s="44"/>
       <c r="S13" s="45"/>
     </row>
-    <row r="14" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B14" s="63"/>
-      <c r="C14" s="65"/>
+    <row r="14" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="65"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="28" t="s">
         <v>14</v>
       </c>
@@ -1232,11 +1246,11 @@
       <c r="R14" s="44"/>
       <c r="S14" s="45"/>
     </row>
-    <row r="15" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B15" s="64" t="s">
+    <row r="15" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="66" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="27" t="s">
@@ -1258,9 +1272,9 @@
       <c r="R15" s="44"/>
       <c r="S15" s="45"/>
     </row>
-    <row r="16" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
+    <row r="16" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="28" t="s">
         <v>14</v>
       </c>
@@ -1280,11 +1294,11 @@
       <c r="R16" s="44"/>
       <c r="S16" s="45"/>
     </row>
-    <row r="17" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B17" s="64" t="s">
+    <row r="17" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="66" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="27" t="s">
@@ -1306,9 +1320,9 @@
       <c r="R17" s="44"/>
       <c r="S17" s="45"/>
     </row>
-    <row r="18" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
+    <row r="18" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="28" t="s">
         <v>14</v>
       </c>
@@ -1328,11 +1342,11 @@
       <c r="R18" s="44"/>
       <c r="S18" s="45"/>
     </row>
-    <row r="19" spans="2:19" ht="14.4">
-      <c r="B19" s="64" t="s">
+    <row r="19" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B19" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="27" t="s">
@@ -1354,9 +1368,9 @@
       <c r="R19" s="44"/>
       <c r="S19" s="45"/>
     </row>
-    <row r="20" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
+    <row r="20" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="28" t="s">
         <v>14</v>
       </c>
@@ -1376,11 +1390,11 @@
       <c r="R20" s="44"/>
       <c r="S20" s="45"/>
     </row>
-    <row r="21" spans="2:19" ht="14.4">
-      <c r="B21" s="64" t="s">
+    <row r="21" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B21" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="66" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="27" t="s">
@@ -1402,9 +1416,9 @@
       <c r="R21" s="44"/>
       <c r="S21" s="45"/>
     </row>
-    <row r="22" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
+    <row r="22" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="28" t="s">
         <v>14</v>
       </c>
@@ -1414,7 +1428,7 @@
       <c r="H22" s="51"/>
       <c r="I22" s="51"/>
       <c r="J22" s="52"/>
-      <c r="K22" s="43"/>
+      <c r="K22" s="74"/>
       <c r="L22" s="53"/>
       <c r="M22" s="45"/>
       <c r="N22" s="41"/>
@@ -1424,11 +1438,11 @@
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
-    <row r="23" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B23" s="64" t="s">
+    <row r="23" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="66" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="27" t="s">
@@ -1450,9 +1464,9 @@
       <c r="R23" s="44"/>
       <c r="S23" s="45"/>
     </row>
-    <row r="24" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
+    <row r="24" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="28" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1476,7 @@
       <c r="H24" s="51"/>
       <c r="I24" s="51"/>
       <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
+      <c r="K24" s="61"/>
       <c r="L24" s="44"/>
       <c r="M24" s="45"/>
       <c r="N24" s="41"/>
@@ -1472,11 +1486,11 @@
       <c r="R24" s="44"/>
       <c r="S24" s="45"/>
     </row>
-    <row r="25" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B25" s="62" t="s">
+    <row r="25" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="64" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="27" t="s">
@@ -1498,9 +1512,9 @@
       <c r="R25" s="44"/>
       <c r="S25" s="45"/>
     </row>
-    <row r="26" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
+    <row r="26" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="28" t="s">
         <v>14</v>
       </c>
@@ -1520,11 +1534,11 @@
       <c r="R26" s="44"/>
       <c r="S26" s="45"/>
     </row>
-    <row r="27" spans="2:19" ht="14.4">
-      <c r="B27" s="62" t="s">
+    <row r="27" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B27" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="62" t="s">
+      <c r="C27" s="64" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="27" t="s">
@@ -1546,19 +1560,19 @@
       <c r="R27" s="44"/>
       <c r="S27" s="45"/>
     </row>
-    <row r="28" spans="2:19" ht="14.55" customHeight="1">
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
+    <row r="28" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
-      <c r="H28" s="72"/>
+      <c r="H28" s="62"/>
       <c r="I28" s="48"/>
       <c r="J28" s="48"/>
-      <c r="K28" s="73"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="53"/>
       <c r="M28" s="54"/>
       <c r="N28" s="55"/>
@@ -1568,11 +1582,11 @@
       <c r="R28" s="44"/>
       <c r="S28" s="45"/>
     </row>
-    <row r="29" spans="2:19" ht="14.4">
-      <c r="B29" s="62" t="s">
+    <row r="29" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B29" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="64" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="27" t="s">
@@ -1594,9 +1608,9 @@
       <c r="R29" s="53"/>
       <c r="S29" s="45"/>
     </row>
-    <row r="30" spans="2:19" ht="15" customHeight="1">
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
+    <row r="30" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="28" t="s">
         <v>14</v>
       </c>
@@ -1616,11 +1630,11 @@
       <c r="R30" s="44"/>
       <c r="S30" s="45"/>
     </row>
-    <row r="31" spans="2:19" ht="15" customHeight="1">
-      <c r="B31" s="62" t="s">
+    <row r="31" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="27" t="s">
@@ -1642,9 +1656,9 @@
       <c r="R31" s="42"/>
       <c r="S31" s="45"/>
     </row>
-    <row r="32" spans="2:19" ht="15" customHeight="1">
-      <c r="B32" s="63"/>
-      <c r="C32" s="65"/>
+    <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="65"/>
+      <c r="C32" s="67"/>
       <c r="D32" s="28" t="s">
         <v>14</v>
       </c>
@@ -1664,10 +1678,21 @@
       <c r="R32" s="51"/>
       <c r="S32" s="45"/>
     </row>
-    <row r="34" ht="14.4"/>
-    <row r="35" ht="14.4"/>
+    <row r="34" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D5:M5"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B27:B28"/>
@@ -1683,17 +1708,6 @@
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D5:M5"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C27:C28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>